<commit_message>
Added CartPage methods, properties cleaned up, UniquID method transfered to ExcelUtils.
</commit_message>
<xml_diff>
--- a/ITBootcamp_Final_Project/data/pet-store-data.xlsx
+++ b/ITBootcamp_Final_Project/data/pet-store-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="615">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1710,6 +1710,156 @@
   </si>
   <si>
     <t>af95481</t>
+  </si>
+  <si>
+    <t>b554cb5</t>
+  </si>
+  <si>
+    <t>a24a28d</t>
+  </si>
+  <si>
+    <t>3b458f7</t>
+  </si>
+  <si>
+    <t>1bea8b2</t>
+  </si>
+  <si>
+    <t>535ca68</t>
+  </si>
+  <si>
+    <t>8257ed5</t>
+  </si>
+  <si>
+    <t>50bff96</t>
+  </si>
+  <si>
+    <t>8881302</t>
+  </si>
+  <si>
+    <t>8d9ceb0</t>
+  </si>
+  <si>
+    <t>5884be1</t>
+  </si>
+  <si>
+    <t>db7e18d</t>
+  </si>
+  <si>
+    <t>0eccbea</t>
+  </si>
+  <si>
+    <t>cac0364</t>
+  </si>
+  <si>
+    <t>a411821</t>
+  </si>
+  <si>
+    <t>bc3c93f</t>
+  </si>
+  <si>
+    <t>782bdc2</t>
+  </si>
+  <si>
+    <t>764abe1</t>
+  </si>
+  <si>
+    <t>2298935</t>
+  </si>
+  <si>
+    <t>b8b4d88</t>
+  </si>
+  <si>
+    <t>b635fb7</t>
+  </si>
+  <si>
+    <t>fbdf7f0</t>
+  </si>
+  <si>
+    <t>5fc7519</t>
+  </si>
+  <si>
+    <t>fbc3c63</t>
+  </si>
+  <si>
+    <t>44c3b59</t>
+  </si>
+  <si>
+    <t>a81c662</t>
+  </si>
+  <si>
+    <t>2cd2b92</t>
+  </si>
+  <si>
+    <t>a5efbd7</t>
+  </si>
+  <si>
+    <t>c297cc2</t>
+  </si>
+  <si>
+    <t>f0aeb17</t>
+  </si>
+  <si>
+    <t>00f89a0</t>
+  </si>
+  <si>
+    <t>d08d124</t>
+  </si>
+  <si>
+    <t>b6d380f</t>
+  </si>
+  <si>
+    <t>e3dbb90</t>
+  </si>
+  <si>
+    <t>aff06c9</t>
+  </si>
+  <si>
+    <t>7540dcc</t>
+  </si>
+  <si>
+    <t>a806d69</t>
+  </si>
+  <si>
+    <t>015ec49</t>
+  </si>
+  <si>
+    <t>5615e04</t>
+  </si>
+  <si>
+    <t>e73a78d</t>
+  </si>
+  <si>
+    <t>ead35c7</t>
+  </si>
+  <si>
+    <t>897b4eb</t>
+  </si>
+  <si>
+    <t>a679e19</t>
+  </si>
+  <si>
+    <t>b935cb5</t>
+  </si>
+  <si>
+    <t>7fdf5a3</t>
+  </si>
+  <si>
+    <t>eb048e7</t>
+  </si>
+  <si>
+    <t>3ad3244</t>
+  </si>
+  <si>
+    <t>6f4f49b</t>
+  </si>
+  <si>
+    <t>4e4b33c</t>
+  </si>
+  <si>
+    <t>89114a0</t>
+  </si>
+  <si>
+    <t>d29a4fa</t>
   </si>
 </sst>
 </file>
@@ -2346,7 +2496,7 @@
     </row>
     <row r="2" spans="1:12" ht="44.25" thickBot="1">
       <c r="A2" s="4" t="s">
-        <v>515</v>
+        <v>565</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -2384,7 +2534,7 @@
     </row>
     <row r="3" spans="1:12" ht="44.25" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>516</v>
+        <v>566</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -2422,7 +2572,7 @@
     </row>
     <row r="4" spans="1:12" ht="58.5" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>517</v>
+        <v>567</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -2460,7 +2610,7 @@
     </row>
     <row r="5" spans="1:12" ht="58.5" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>518</v>
+        <v>568</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -2498,7 +2648,7 @@
     </row>
     <row r="6" spans="1:12" ht="44.25" thickBot="1">
       <c r="A6" s="4" t="s">
-        <v>519</v>
+        <v>569</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -2536,7 +2686,7 @@
     </row>
     <row r="7" spans="1:12" ht="44.25" thickBot="1">
       <c r="A7" s="7" t="s">
-        <v>520</v>
+        <v>570</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -2574,7 +2724,7 @@
     </row>
     <row r="8" spans="1:12" ht="44.25" thickBot="1">
       <c r="A8" s="4" t="s">
-        <v>521</v>
+        <v>571</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -2612,7 +2762,7 @@
     </row>
     <row r="9" spans="1:12" ht="44.25" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>522</v>
+        <v>572</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -2650,7 +2800,7 @@
     </row>
     <row r="10" spans="1:12" ht="58.5" thickBot="1">
       <c r="A10" s="7" t="s">
-        <v>523</v>
+        <v>573</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -2688,7 +2838,7 @@
     </row>
     <row r="11" spans="1:12" ht="58.5" thickBot="1">
       <c r="A11" s="4" t="s">
-        <v>524</v>
+        <v>574</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -2726,7 +2876,7 @@
     </row>
     <row r="12" spans="1:12" ht="58.5" thickBot="1">
       <c r="A12" s="4" t="s">
-        <v>525</v>
+        <v>575</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -2764,7 +2914,7 @@
     </row>
     <row r="13" spans="1:12" ht="44.25" thickBot="1">
       <c r="A13" s="7" t="s">
-        <v>526</v>
+        <v>576</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -2802,7 +2952,7 @@
     </row>
     <row r="14" spans="1:12" ht="44.25" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>527</v>
+        <v>577</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -2840,7 +2990,7 @@
     </row>
     <row r="15" spans="1:12" ht="44.25" thickBot="1">
       <c r="A15" s="4" t="s">
-        <v>528</v>
+        <v>578</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -2878,7 +3028,7 @@
     </row>
     <row r="16" spans="1:12" ht="44.25" thickBot="1">
       <c r="A16" s="7" t="s">
-        <v>529</v>
+        <v>579</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -2916,7 +3066,7 @@
     </row>
     <row r="17" spans="1:12" ht="44.25" thickBot="1">
       <c r="A17" s="4" t="s">
-        <v>530</v>
+        <v>580</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -2954,7 +3104,7 @@
     </row>
     <row r="18" spans="1:12" ht="44.25" thickBot="1">
       <c r="A18" s="4" t="s">
-        <v>531</v>
+        <v>581</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -2992,7 +3142,7 @@
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1">
       <c r="A19" s="7" t="s">
-        <v>532</v>
+        <v>582</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -3030,7 +3180,7 @@
     </row>
     <row r="20" spans="1:12" ht="44.25" thickBot="1">
       <c r="A20" s="4" t="s">
-        <v>533</v>
+        <v>583</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -3068,7 +3218,7 @@
     </row>
     <row r="21" spans="1:12" ht="44.25" thickBot="1">
       <c r="A21" s="4" t="s">
-        <v>534</v>
+        <v>584</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -3106,7 +3256,7 @@
     </row>
     <row r="22" spans="1:12" ht="44.25" thickBot="1">
       <c r="A22" s="7" t="s">
-        <v>535</v>
+        <v>585</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -3144,7 +3294,7 @@
     </row>
     <row r="23" spans="1:12" ht="58.5" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>536</v>
+        <v>586</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -3182,7 +3332,7 @@
     </row>
     <row r="24" spans="1:12" ht="44.25" thickBot="1">
       <c r="A24" s="4" t="s">
-        <v>537</v>
+        <v>587</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -3220,7 +3370,7 @@
     </row>
     <row r="25" spans="1:12" ht="58.5" thickBot="1">
       <c r="A25" s="7" t="s">
-        <v>538</v>
+        <v>588</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -3258,7 +3408,7 @@
     </row>
     <row r="26" spans="1:12" ht="58.5" thickBot="1">
       <c r="A26" s="4" t="s">
-        <v>539</v>
+        <v>589</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -3296,7 +3446,7 @@
     </row>
     <row r="27" spans="1:12" ht="58.5" thickBot="1">
       <c r="A27" s="4" t="s">
-        <v>540</v>
+        <v>590</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -3334,7 +3484,7 @@
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1">
       <c r="A28" s="7" t="s">
-        <v>541</v>
+        <v>591</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -3372,7 +3522,7 @@
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1">
       <c r="A29" s="4" t="s">
-        <v>542</v>
+        <v>592</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -3410,7 +3560,7 @@
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1">
       <c r="A30" s="4" t="s">
-        <v>543</v>
+        <v>593</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -3448,7 +3598,7 @@
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1">
       <c r="A31" s="7" t="s">
-        <v>544</v>
+        <v>594</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -3486,7 +3636,7 @@
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1">
       <c r="A32" s="4" t="s">
-        <v>545</v>
+        <v>595</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -3524,7 +3674,7 @@
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1">
       <c r="A33" s="4" t="s">
-        <v>546</v>
+        <v>596</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -3562,7 +3712,7 @@
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1">
       <c r="A34" s="7" t="s">
-        <v>547</v>
+        <v>597</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -3600,7 +3750,7 @@
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1">
       <c r="A35" s="4" t="s">
-        <v>548</v>
+        <v>598</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -3638,7 +3788,7 @@
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1">
       <c r="A36" s="4" t="s">
-        <v>549</v>
+        <v>599</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -3676,7 +3826,7 @@
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1">
       <c r="A37" s="7" t="s">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -3714,7 +3864,7 @@
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1">
       <c r="A38" s="4" t="s">
-        <v>551</v>
+        <v>601</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -3752,7 +3902,7 @@
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1">
       <c r="A39" s="4" t="s">
-        <v>552</v>
+        <v>602</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -3790,7 +3940,7 @@
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1">
       <c r="A40" s="7" t="s">
-        <v>553</v>
+        <v>603</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -3828,7 +3978,7 @@
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1">
       <c r="A41" s="4" t="s">
-        <v>554</v>
+        <v>604</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -3866,7 +4016,7 @@
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1">
       <c r="A42" s="4" t="s">
-        <v>555</v>
+        <v>605</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -3904,7 +4054,7 @@
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1">
       <c r="A43" s="7" t="s">
-        <v>556</v>
+        <v>606</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -3942,7 +4092,7 @@
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1">
       <c r="A44" s="4" t="s">
-        <v>557</v>
+        <v>607</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -3980,7 +4130,7 @@
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1">
       <c r="A45" s="4" t="s">
-        <v>558</v>
+        <v>608</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -4018,7 +4168,7 @@
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1">
       <c r="A46" s="7" t="s">
-        <v>559</v>
+        <v>609</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -4056,7 +4206,7 @@
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1">
       <c r="A47" s="4" t="s">
-        <v>560</v>
+        <v>610</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -4094,7 +4244,7 @@
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1">
       <c r="A48" s="4" t="s">
-        <v>561</v>
+        <v>611</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -4132,7 +4282,7 @@
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1">
       <c r="A49" s="7" t="s">
-        <v>562</v>
+        <v>612</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -4170,7 +4320,7 @@
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1">
       <c r="A50" s="4" t="s">
-        <v>563</v>
+        <v>613</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -4208,7 +4358,7 @@
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1">
       <c r="A51" s="4" t="s">
-        <v>564</v>
+        <v>614</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>

</xml_diff>

<commit_message>
Add methods to ExcelUtils, completed RegistrationPage, edited some page
</commit_message>
<xml_diff>
--- a/ITBootcamp_Final_Project/data/pet-store-data.xlsx
+++ b/ITBootcamp_Final_Project/data/pet-store-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="772">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -1860,6 +1860,477 @@
   </si>
   <si>
     <t>d29a4fa</t>
+  </si>
+  <si>
+    <t>2fb3ff2</t>
+  </si>
+  <si>
+    <t>2db9f93</t>
+  </si>
+  <si>
+    <t>8d5f735</t>
+  </si>
+  <si>
+    <t>7287254</t>
+  </si>
+  <si>
+    <t>3a2b5df</t>
+  </si>
+  <si>
+    <t>1bd7ea8</t>
+  </si>
+  <si>
+    <t>138607c</t>
+  </si>
+  <si>
+    <t>928a390</t>
+  </si>
+  <si>
+    <t>60373c2</t>
+  </si>
+  <si>
+    <t>de21e38</t>
+  </si>
+  <si>
+    <t>0af1f07</t>
+  </si>
+  <si>
+    <t>8314644</t>
+  </si>
+  <si>
+    <t>37c2da0</t>
+  </si>
+  <si>
+    <t>a5da979</t>
+  </si>
+  <si>
+    <t>53b9104</t>
+  </si>
+  <si>
+    <t>8023f5e</t>
+  </si>
+  <si>
+    <t>01f3e35</t>
+  </si>
+  <si>
+    <t>b46defd</t>
+  </si>
+  <si>
+    <t>fe0a19a</t>
+  </si>
+  <si>
+    <t>0b03b6a</t>
+  </si>
+  <si>
+    <t>364f0f2</t>
+  </si>
+  <si>
+    <t>337abdd</t>
+  </si>
+  <si>
+    <t>193ede0</t>
+  </si>
+  <si>
+    <t>927dffe</t>
+  </si>
+  <si>
+    <t>dd13c2c</t>
+  </si>
+  <si>
+    <t>ce07a64</t>
+  </si>
+  <si>
+    <t>13d449a</t>
+  </si>
+  <si>
+    <t>7296892</t>
+  </si>
+  <si>
+    <t>928bab4</t>
+  </si>
+  <si>
+    <t>8fbac55</t>
+  </si>
+  <si>
+    <t>7d8547b</t>
+  </si>
+  <si>
+    <t>8691ce3</t>
+  </si>
+  <si>
+    <t>979d631</t>
+  </si>
+  <si>
+    <t>b1e1236</t>
+  </si>
+  <si>
+    <t>afeebeb</t>
+  </si>
+  <si>
+    <t>245cfb3</t>
+  </si>
+  <si>
+    <t>e5d021e</t>
+  </si>
+  <si>
+    <t>008f6e4</t>
+  </si>
+  <si>
+    <t>9e247bd</t>
+  </si>
+  <si>
+    <t>22cd863</t>
+  </si>
+  <si>
+    <t>a0493ed</t>
+  </si>
+  <si>
+    <t>11ff0a4</t>
+  </si>
+  <si>
+    <t>04aac14</t>
+  </si>
+  <si>
+    <t>85a3c79</t>
+  </si>
+  <si>
+    <t>27d39b9</t>
+  </si>
+  <si>
+    <t>91c8cbd</t>
+  </si>
+  <si>
+    <t>b72d152</t>
+  </si>
+  <si>
+    <t>966894a</t>
+  </si>
+  <si>
+    <t>45e5785</t>
+  </si>
+  <si>
+    <t>b5019df</t>
+  </si>
+  <si>
+    <t>0e89eef</t>
+  </si>
+  <si>
+    <t>01a00d6</t>
+  </si>
+  <si>
+    <t>5b9a47f</t>
+  </si>
+  <si>
+    <t>307394e</t>
+  </si>
+  <si>
+    <t>0b6f97f</t>
+  </si>
+  <si>
+    <t>bfc14a9</t>
+  </si>
+  <si>
+    <t>d3bbd95</t>
+  </si>
+  <si>
+    <t>accf343</t>
+  </si>
+  <si>
+    <t>508e4a7</t>
+  </si>
+  <si>
+    <t>1b57bda</t>
+  </si>
+  <si>
+    <t>325a21c</t>
+  </si>
+  <si>
+    <t>a000677</t>
+  </si>
+  <si>
+    <t>5f8de2b</t>
+  </si>
+  <si>
+    <t>3199e15</t>
+  </si>
+  <si>
+    <t>8b9570b</t>
+  </si>
+  <si>
+    <t>94a6f71</t>
+  </si>
+  <si>
+    <t>b5ec507</t>
+  </si>
+  <si>
+    <t>73f10b3</t>
+  </si>
+  <si>
+    <t>e0a4b12</t>
+  </si>
+  <si>
+    <t>71b060f</t>
+  </si>
+  <si>
+    <t>22de005</t>
+  </si>
+  <si>
+    <t>d38cc4a</t>
+  </si>
+  <si>
+    <t>bb71770</t>
+  </si>
+  <si>
+    <t>0cc29a4</t>
+  </si>
+  <si>
+    <t>ebaf605</t>
+  </si>
+  <si>
+    <t>7c9aa29</t>
+  </si>
+  <si>
+    <t>5cda996</t>
+  </si>
+  <si>
+    <t>e25bc73</t>
+  </si>
+  <si>
+    <t>41d9c81</t>
+  </si>
+  <si>
+    <t>1877776</t>
+  </si>
+  <si>
+    <t>810a132</t>
+  </si>
+  <si>
+    <t>d4c50cc</t>
+  </si>
+  <si>
+    <t>1e32338</t>
+  </si>
+  <si>
+    <t>4875662</t>
+  </si>
+  <si>
+    <t>6eb3440</t>
+  </si>
+  <si>
+    <t>f0d0046</t>
+  </si>
+  <si>
+    <t>d1e5a93</t>
+  </si>
+  <si>
+    <t>e56b85d</t>
+  </si>
+  <si>
+    <t>77645d0</t>
+  </si>
+  <si>
+    <t>3a0adfd</t>
+  </si>
+  <si>
+    <t>58ab93b</t>
+  </si>
+  <si>
+    <t>9d2b899</t>
+  </si>
+  <si>
+    <t>50bc0ac</t>
+  </si>
+  <si>
+    <t>91e2c6e</t>
+  </si>
+  <si>
+    <t>e38673e</t>
+  </si>
+  <si>
+    <t>253c87c</t>
+  </si>
+  <si>
+    <t>8a44099</t>
+  </si>
+  <si>
+    <t>9f723a1</t>
+  </si>
+  <si>
+    <t>f164641</t>
+  </si>
+  <si>
+    <t>bf78a03</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>japanese</t>
+  </si>
+  <si>
+    <t>FISH</t>
+  </si>
+  <si>
+    <t>CATS</t>
+  </si>
+  <si>
+    <t>REPTILES</t>
+  </si>
+  <si>
+    <t>BIRDS</t>
+  </si>
+  <si>
+    <t>DOGS</t>
+  </si>
+  <si>
+    <t>6ec6865</t>
+  </si>
+  <si>
+    <t>e171a8c</t>
+  </si>
+  <si>
+    <t>36f4b27</t>
+  </si>
+  <si>
+    <t>a97b0c0</t>
+  </si>
+  <si>
+    <t>7bb2994</t>
+  </si>
+  <si>
+    <t>77fe59a</t>
+  </si>
+  <si>
+    <t>84c1063</t>
+  </si>
+  <si>
+    <t>3b1030c</t>
+  </si>
+  <si>
+    <t>7037844</t>
+  </si>
+  <si>
+    <t>2898a3d</t>
+  </si>
+  <si>
+    <t>968ac2c</t>
+  </si>
+  <si>
+    <t>2f69c54</t>
+  </si>
+  <si>
+    <t>57a6843</t>
+  </si>
+  <si>
+    <t>ab28c27</t>
+  </si>
+  <si>
+    <t>e4dbdd0</t>
+  </si>
+  <si>
+    <t>8093fc0</t>
+  </si>
+  <si>
+    <t>c748cbe</t>
+  </si>
+  <si>
+    <t>bf63886</t>
+  </si>
+  <si>
+    <t>ac53d9d</t>
+  </si>
+  <si>
+    <t>00b6a67</t>
+  </si>
+  <si>
+    <t>f74faa2</t>
+  </si>
+  <si>
+    <t>567b681</t>
+  </si>
+  <si>
+    <t>e00541f</t>
+  </si>
+  <si>
+    <t>33a8dbf</t>
+  </si>
+  <si>
+    <t>facd836</t>
+  </si>
+  <si>
+    <t>8bc788b</t>
+  </si>
+  <si>
+    <t>04355de</t>
+  </si>
+  <si>
+    <t>e980e07</t>
+  </si>
+  <si>
+    <t>846dcd7</t>
+  </si>
+  <si>
+    <t>b63f931</t>
+  </si>
+  <si>
+    <t>0546833</t>
+  </si>
+  <si>
+    <t>ba118b7</t>
+  </si>
+  <si>
+    <t>e4f6ed2</t>
+  </si>
+  <si>
+    <t>f6cb6c6</t>
+  </si>
+  <si>
+    <t>1da3d85</t>
+  </si>
+  <si>
+    <t>39f8369</t>
+  </si>
+  <si>
+    <t>620936b</t>
+  </si>
+  <si>
+    <t>176b83d</t>
+  </si>
+  <si>
+    <t>2e43780</t>
+  </si>
+  <si>
+    <t>d8b1f35</t>
+  </si>
+  <si>
+    <t>41c1b48</t>
+  </si>
+  <si>
+    <t>1b661e3</t>
+  </si>
+  <si>
+    <t>8c27037</t>
+  </si>
+  <si>
+    <t>97f6b44</t>
+  </si>
+  <si>
+    <t>e62fce7</t>
+  </si>
+  <si>
+    <t>43b0e64</t>
+  </si>
+  <si>
+    <t>eb3c276</t>
+  </si>
+  <si>
+    <t>fe00d75</t>
+  </si>
+  <si>
+    <t>223353f</t>
+  </si>
+  <si>
+    <t>4409c48</t>
   </si>
 </sst>
 </file>
@@ -2441,7 +2912,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -2496,7 +2967,7 @@
     </row>
     <row r="2" spans="1:12" ht="44.25" thickBot="1">
       <c r="A2" s="4" t="s">
-        <v>565</v>
+        <v>722</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -2531,10 +3002,16 @@
       <c r="L2" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M2" t="s">
+        <v>715</v>
+      </c>
+      <c r="N2" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="44.25" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>566</v>
+        <v>723</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -2569,10 +3046,16 @@
       <c r="L3" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M3" t="s">
+        <v>715</v>
+      </c>
+      <c r="N3" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="58.5" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>567</v>
+        <v>724</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -2607,10 +3090,16 @@
       <c r="L4" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M4" t="s">
+        <v>716</v>
+      </c>
+      <c r="N4" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="58.5" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>568</v>
+        <v>725</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -2645,10 +3134,16 @@
       <c r="L5" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M5" t="s">
+        <v>715</v>
+      </c>
+      <c r="N5" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="44.25" thickBot="1">
       <c r="A6" s="4" t="s">
-        <v>569</v>
+        <v>726</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -2683,10 +3178,16 @@
       <c r="L6" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M6" t="s">
+        <v>715</v>
+      </c>
+      <c r="N6" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="44.25" thickBot="1">
       <c r="A7" s="7" t="s">
-        <v>570</v>
+        <v>727</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -2721,10 +3222,16 @@
       <c r="L7" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M7" t="s">
+        <v>716</v>
+      </c>
+      <c r="N7" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="44.25" thickBot="1">
       <c r="A8" s="4" t="s">
-        <v>571</v>
+        <v>728</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -2759,10 +3266,16 @@
       <c r="L8" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M8" t="s">
+        <v>716</v>
+      </c>
+      <c r="N8" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="44.25" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>572</v>
+        <v>729</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -2797,10 +3310,16 @@
       <c r="L9" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M9" t="s">
+        <v>716</v>
+      </c>
+      <c r="N9" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="58.5" thickBot="1">
       <c r="A10" s="7" t="s">
-        <v>573</v>
+        <v>730</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -2835,10 +3354,16 @@
       <c r="L10" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M10" t="s">
+        <v>715</v>
+      </c>
+      <c r="N10" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="58.5" thickBot="1">
       <c r="A11" s="4" t="s">
-        <v>574</v>
+        <v>731</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -2873,10 +3398,16 @@
       <c r="L11" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M11" t="s">
+        <v>715</v>
+      </c>
+      <c r="N11" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="58.5" thickBot="1">
       <c r="A12" s="4" t="s">
-        <v>575</v>
+        <v>732</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -2911,10 +3442,16 @@
       <c r="L12" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M12" t="s">
+        <v>715</v>
+      </c>
+      <c r="N12" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="44.25" thickBot="1">
       <c r="A13" s="7" t="s">
-        <v>576</v>
+        <v>733</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -2949,10 +3486,16 @@
       <c r="L13" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M13" t="s">
+        <v>715</v>
+      </c>
+      <c r="N13" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="44.25" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>577</v>
+        <v>734</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -2987,10 +3530,16 @@
       <c r="L14" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M14" t="s">
+        <v>716</v>
+      </c>
+      <c r="N14" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="44.25" thickBot="1">
       <c r="A15" s="4" t="s">
-        <v>578</v>
+        <v>735</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -3025,10 +3574,16 @@
       <c r="L15" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M15" t="s">
+        <v>715</v>
+      </c>
+      <c r="N15" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="44.25" thickBot="1">
       <c r="A16" s="7" t="s">
-        <v>579</v>
+        <v>736</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -3063,10 +3618,16 @@
       <c r="L16" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M16" t="s">
+        <v>715</v>
+      </c>
+      <c r="N16" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="44.25" thickBot="1">
       <c r="A17" s="4" t="s">
-        <v>580</v>
+        <v>737</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -3101,10 +3662,16 @@
       <c r="L17" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M17" t="s">
+        <v>715</v>
+      </c>
+      <c r="N17" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="44.25" thickBot="1">
       <c r="A18" s="4" t="s">
-        <v>581</v>
+        <v>738</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -3139,10 +3706,16 @@
       <c r="L18" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M18" t="s">
+        <v>715</v>
+      </c>
+      <c r="N18" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1">
       <c r="A19" s="7" t="s">
-        <v>582</v>
+        <v>739</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -3177,10 +3750,16 @@
       <c r="L19" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M19" t="s">
+        <v>715</v>
+      </c>
+      <c r="N19" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="44.25" thickBot="1">
       <c r="A20" s="4" t="s">
-        <v>583</v>
+        <v>740</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -3215,10 +3794,16 @@
       <c r="L20" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M20" t="s">
+        <v>716</v>
+      </c>
+      <c r="N20" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="44.25" thickBot="1">
       <c r="A21" s="4" t="s">
-        <v>584</v>
+        <v>741</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -3253,10 +3838,16 @@
       <c r="L21" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M21" t="s">
+        <v>715</v>
+      </c>
+      <c r="N21" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="44.25" thickBot="1">
       <c r="A22" s="7" t="s">
-        <v>585</v>
+        <v>742</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -3291,10 +3882,16 @@
       <c r="L22" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M22" t="s">
+        <v>715</v>
+      </c>
+      <c r="N22" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="23" spans="1:12" ht="58.5" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>586</v>
+        <v>743</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -3329,10 +3926,16 @@
       <c r="L23" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M23" t="s">
+        <v>715</v>
+      </c>
+      <c r="N23" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="44.25" thickBot="1">
       <c r="A24" s="4" t="s">
-        <v>587</v>
+        <v>744</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -3367,10 +3970,16 @@
       <c r="L24" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M24" t="s">
+        <v>715</v>
+      </c>
+      <c r="N24" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="58.5" thickBot="1">
       <c r="A25" s="7" t="s">
-        <v>588</v>
+        <v>745</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -3405,10 +4014,16 @@
       <c r="L25" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M25" t="s">
+        <v>716</v>
+      </c>
+      <c r="N25" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="58.5" thickBot="1">
       <c r="A26" s="4" t="s">
-        <v>589</v>
+        <v>746</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -3443,10 +4058,16 @@
       <c r="L26" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M26" t="s">
+        <v>715</v>
+      </c>
+      <c r="N26" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="58.5" thickBot="1">
       <c r="A27" s="4" t="s">
-        <v>590</v>
+        <v>747</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -3481,10 +4102,16 @@
       <c r="L27" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M27" t="s">
+        <v>716</v>
+      </c>
+      <c r="N27" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1">
       <c r="A28" s="7" t="s">
-        <v>591</v>
+        <v>748</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -3519,10 +4146,16 @@
       <c r="L28" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M28" t="s">
+        <v>716</v>
+      </c>
+      <c r="N28" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1">
       <c r="A29" s="4" t="s">
-        <v>592</v>
+        <v>749</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -3557,10 +4190,16 @@
       <c r="L29" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M29" t="s">
+        <v>716</v>
+      </c>
+      <c r="N29" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1">
       <c r="A30" s="4" t="s">
-        <v>593</v>
+        <v>750</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -3595,10 +4234,16 @@
       <c r="L30" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M30" t="s">
+        <v>715</v>
+      </c>
+      <c r="N30" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1">
       <c r="A31" s="7" t="s">
-        <v>594</v>
+        <v>751</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -3633,10 +4278,16 @@
       <c r="L31" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M31" t="s">
+        <v>715</v>
+      </c>
+      <c r="N31" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1">
       <c r="A32" s="4" t="s">
-        <v>595</v>
+        <v>752</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -3671,10 +4322,16 @@
       <c r="L32" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M32" t="s">
+        <v>715</v>
+      </c>
+      <c r="N32" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1">
       <c r="A33" s="4" t="s">
-        <v>596</v>
+        <v>753</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -3709,10 +4366,16 @@
       <c r="L33" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M33" t="s">
+        <v>716</v>
+      </c>
+      <c r="N33" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1">
       <c r="A34" s="7" t="s">
-        <v>597</v>
+        <v>754</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -3747,10 +4410,16 @@
       <c r="L34" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M34" t="s">
+        <v>715</v>
+      </c>
+      <c r="N34" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1">
       <c r="A35" s="4" t="s">
-        <v>598</v>
+        <v>755</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -3785,10 +4454,16 @@
       <c r="L35" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M35" t="s">
+        <v>715</v>
+      </c>
+      <c r="N35" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1">
       <c r="A36" s="4" t="s">
-        <v>599</v>
+        <v>756</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -3823,10 +4498,16 @@
       <c r="L36" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M36" t="s">
+        <v>715</v>
+      </c>
+      <c r="N36" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1">
       <c r="A37" s="7" t="s">
-        <v>600</v>
+        <v>757</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -3861,10 +4542,16 @@
       <c r="L37" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M37" t="s">
+        <v>716</v>
+      </c>
+      <c r="N37" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1">
       <c r="A38" s="4" t="s">
-        <v>601</v>
+        <v>758</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -3899,10 +4586,16 @@
       <c r="L38" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M38" t="s">
+        <v>716</v>
+      </c>
+      <c r="N38" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1">
       <c r="A39" s="4" t="s">
-        <v>602</v>
+        <v>759</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -3937,10 +4630,16 @@
       <c r="L39" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M39" t="s">
+        <v>715</v>
+      </c>
+      <c r="N39" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1">
       <c r="A40" s="7" t="s">
-        <v>603</v>
+        <v>760</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -3975,10 +4674,16 @@
       <c r="L40" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M40" t="s">
+        <v>715</v>
+      </c>
+      <c r="N40" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1">
       <c r="A41" s="4" t="s">
-        <v>604</v>
+        <v>761</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -4013,10 +4718,16 @@
       <c r="L41" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M41" t="s">
+        <v>715</v>
+      </c>
+      <c r="N41" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1">
       <c r="A42" s="4" t="s">
-        <v>605</v>
+        <v>762</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -4051,10 +4762,16 @@
       <c r="L42" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M42" t="s">
+        <v>716</v>
+      </c>
+      <c r="N42" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1">
       <c r="A43" s="7" t="s">
-        <v>606</v>
+        <v>763</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -4089,10 +4806,16 @@
       <c r="L43" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M43" t="s">
+        <v>715</v>
+      </c>
+      <c r="N43" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1">
       <c r="A44" s="4" t="s">
-        <v>607</v>
+        <v>764</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -4127,10 +4850,16 @@
       <c r="L44" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M44" t="s">
+        <v>716</v>
+      </c>
+      <c r="N44" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1">
       <c r="A45" s="4" t="s">
-        <v>608</v>
+        <v>765</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -4165,10 +4894,16 @@
       <c r="L45" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M45" t="s">
+        <v>716</v>
+      </c>
+      <c r="N45" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1">
       <c r="A46" s="7" t="s">
-        <v>609</v>
+        <v>766</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -4203,10 +4938,16 @@
       <c r="L46" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M46" t="s">
+        <v>715</v>
+      </c>
+      <c r="N46" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1">
       <c r="A47" s="4" t="s">
-        <v>610</v>
+        <v>767</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -4241,10 +4982,16 @@
       <c r="L47" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M47" t="s">
+        <v>715</v>
+      </c>
+      <c r="N47" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1">
       <c r="A48" s="4" t="s">
-        <v>611</v>
+        <v>768</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -4279,10 +5026,16 @@
       <c r="L48" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M48" t="s">
+        <v>715</v>
+      </c>
+      <c r="N48" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1">
       <c r="A49" s="7" t="s">
-        <v>612</v>
+        <v>769</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -4317,10 +5070,16 @@
       <c r="L49" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M49" t="s">
+        <v>715</v>
+      </c>
+      <c r="N49" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1">
       <c r="A50" s="4" t="s">
-        <v>613</v>
+        <v>770</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -4355,10 +5114,16 @@
       <c r="L50" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="M50" t="s">
+        <v>715</v>
+      </c>
+      <c r="N50" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1">
       <c r="A51" s="4" t="s">
-        <v>614</v>
+        <v>771</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>
@@ -4392,6 +5157,12 @@
       </c>
       <c r="L51" s="5" t="s">
         <v>23</v>
+      </c>
+      <c r="M51" t="s">
+        <v>716</v>
+      </c>
+      <c r="N51" t="s">
+        <v>718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding a .xml file and cross browsing testing feature.
</commit_message>
<xml_diff>
--- a/ITBootcamp_Final_Project/data/pet-store-data.xlsx
+++ b/ITBootcamp_Final_Project/data/pet-store-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="1072">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -2331,6 +2331,906 @@
   </si>
   <si>
     <t>4409c48</t>
+  </si>
+  <si>
+    <t>4b52730</t>
+  </si>
+  <si>
+    <t>279c279</t>
+  </si>
+  <si>
+    <t>8d5b3ab</t>
+  </si>
+  <si>
+    <t>d1aa60f</t>
+  </si>
+  <si>
+    <t>228cfaf</t>
+  </si>
+  <si>
+    <t>fe8d62d</t>
+  </si>
+  <si>
+    <t>f06497b</t>
+  </si>
+  <si>
+    <t>5c19da4</t>
+  </si>
+  <si>
+    <t>92469ed</t>
+  </si>
+  <si>
+    <t>75ffe10</t>
+  </si>
+  <si>
+    <t>12b6ff9</t>
+  </si>
+  <si>
+    <t>3821a80</t>
+  </si>
+  <si>
+    <t>5c84d33</t>
+  </si>
+  <si>
+    <t>17bc13a</t>
+  </si>
+  <si>
+    <t>cb508f2</t>
+  </si>
+  <si>
+    <t>59e8728</t>
+  </si>
+  <si>
+    <t>823908b</t>
+  </si>
+  <si>
+    <t>c9d2cd1</t>
+  </si>
+  <si>
+    <t>001bd29</t>
+  </si>
+  <si>
+    <t>dd90e23</t>
+  </si>
+  <si>
+    <t>1470841</t>
+  </si>
+  <si>
+    <t>55a631c</t>
+  </si>
+  <si>
+    <t>2303f88</t>
+  </si>
+  <si>
+    <t>0cc6f0e</t>
+  </si>
+  <si>
+    <t>497e6f2</t>
+  </si>
+  <si>
+    <t>e15d5cc</t>
+  </si>
+  <si>
+    <t>a11a248</t>
+  </si>
+  <si>
+    <t>e7508af</t>
+  </si>
+  <si>
+    <t>d56994d</t>
+  </si>
+  <si>
+    <t>e905cdd</t>
+  </si>
+  <si>
+    <t>2c9b8c6</t>
+  </si>
+  <si>
+    <t>3e15331</t>
+  </si>
+  <si>
+    <t>e496f68</t>
+  </si>
+  <si>
+    <t>b803095</t>
+  </si>
+  <si>
+    <t>51a9d19</t>
+  </si>
+  <si>
+    <t>404fe70</t>
+  </si>
+  <si>
+    <t>bcc9608</t>
+  </si>
+  <si>
+    <t>b2bcff0</t>
+  </si>
+  <si>
+    <t>a967afc</t>
+  </si>
+  <si>
+    <t>e4ff1a3</t>
+  </si>
+  <si>
+    <t>bef3a17</t>
+  </si>
+  <si>
+    <t>0f56a43</t>
+  </si>
+  <si>
+    <t>d434881</t>
+  </si>
+  <si>
+    <t>80521d4</t>
+  </si>
+  <si>
+    <t>5828b62</t>
+  </si>
+  <si>
+    <t>3c83547</t>
+  </si>
+  <si>
+    <t>bc901b9</t>
+  </si>
+  <si>
+    <t>14f8aa5</t>
+  </si>
+  <si>
+    <t>d8467a7</t>
+  </si>
+  <si>
+    <t>a1f8e38</t>
+  </si>
+  <si>
+    <t>a605c6a</t>
+  </si>
+  <si>
+    <t>d0b8d66</t>
+  </si>
+  <si>
+    <t>7f1ff71</t>
+  </si>
+  <si>
+    <t>98f6c6b</t>
+  </si>
+  <si>
+    <t>0506304</t>
+  </si>
+  <si>
+    <t>a9c4f5b</t>
+  </si>
+  <si>
+    <t>78feed0</t>
+  </si>
+  <si>
+    <t>9d9b944</t>
+  </si>
+  <si>
+    <t>5ea17fb</t>
+  </si>
+  <si>
+    <t>f0fecb9</t>
+  </si>
+  <si>
+    <t>b939805</t>
+  </si>
+  <si>
+    <t>796978c</t>
+  </si>
+  <si>
+    <t>634e7bc</t>
+  </si>
+  <si>
+    <t>7792d98</t>
+  </si>
+  <si>
+    <t>2f1a1b6</t>
+  </si>
+  <si>
+    <t>fcb7ccd</t>
+  </si>
+  <si>
+    <t>ce3bc90</t>
+  </si>
+  <si>
+    <t>0d61abe</t>
+  </si>
+  <si>
+    <t>8d32c0f</t>
+  </si>
+  <si>
+    <t>4a2b2dd</t>
+  </si>
+  <si>
+    <t>a5f4275</t>
+  </si>
+  <si>
+    <t>2f0c7d2</t>
+  </si>
+  <si>
+    <t>d289662</t>
+  </si>
+  <si>
+    <t>61ce68f</t>
+  </si>
+  <si>
+    <t>f14d1ba</t>
+  </si>
+  <si>
+    <t>22c468b</t>
+  </si>
+  <si>
+    <t>6143734</t>
+  </si>
+  <si>
+    <t>2bdb076</t>
+  </si>
+  <si>
+    <t>3f36f91</t>
+  </si>
+  <si>
+    <t>784b43d</t>
+  </si>
+  <si>
+    <t>154da80</t>
+  </si>
+  <si>
+    <t>ae8fb15</t>
+  </si>
+  <si>
+    <t>41c2119</t>
+  </si>
+  <si>
+    <t>7b053fd</t>
+  </si>
+  <si>
+    <t>d0e68da</t>
+  </si>
+  <si>
+    <t>a14cddd</t>
+  </si>
+  <si>
+    <t>d10b127</t>
+  </si>
+  <si>
+    <t>4efba9d</t>
+  </si>
+  <si>
+    <t>abf054b</t>
+  </si>
+  <si>
+    <t>d15fdf9</t>
+  </si>
+  <si>
+    <t>a255ba2</t>
+  </si>
+  <si>
+    <t>4bc4ccf</t>
+  </si>
+  <si>
+    <t>d23c7f8</t>
+  </si>
+  <si>
+    <t>13e50e6</t>
+  </si>
+  <si>
+    <t>4823dc2</t>
+  </si>
+  <si>
+    <t>6a534c4</t>
+  </si>
+  <si>
+    <t>dc1d591</t>
+  </si>
+  <si>
+    <t>eacef85</t>
+  </si>
+  <si>
+    <t>84c9222</t>
+  </si>
+  <si>
+    <t>32a962e</t>
+  </si>
+  <si>
+    <t>2d79803</t>
+  </si>
+  <si>
+    <t>7b31669</t>
+  </si>
+  <si>
+    <t>c4fb988</t>
+  </si>
+  <si>
+    <t>eea8f1d</t>
+  </si>
+  <si>
+    <t>fd282cd</t>
+  </si>
+  <si>
+    <t>891c463</t>
+  </si>
+  <si>
+    <t>f4126ce</t>
+  </si>
+  <si>
+    <t>38f6f11</t>
+  </si>
+  <si>
+    <t>d070646</t>
+  </si>
+  <si>
+    <t>047ef83</t>
+  </si>
+  <si>
+    <t>db520fe</t>
+  </si>
+  <si>
+    <t>f115f0e</t>
+  </si>
+  <si>
+    <t>b67cff5</t>
+  </si>
+  <si>
+    <t>5b8a111</t>
+  </si>
+  <si>
+    <t>54d2b8e</t>
+  </si>
+  <si>
+    <t>a63bd1d</t>
+  </si>
+  <si>
+    <t>b390bd5</t>
+  </si>
+  <si>
+    <t>143df9b</t>
+  </si>
+  <si>
+    <t>525a19a</t>
+  </si>
+  <si>
+    <t>9f5ecc1</t>
+  </si>
+  <si>
+    <t>11867a3</t>
+  </si>
+  <si>
+    <t>6a96f19</t>
+  </si>
+  <si>
+    <t>d71a077</t>
+  </si>
+  <si>
+    <t>312af17</t>
+  </si>
+  <si>
+    <t>58dac69</t>
+  </si>
+  <si>
+    <t>c0051ed</t>
+  </si>
+  <si>
+    <t>994a212</t>
+  </si>
+  <si>
+    <t>9718034</t>
+  </si>
+  <si>
+    <t>cec66b0</t>
+  </si>
+  <si>
+    <t>e00fc62</t>
+  </si>
+  <si>
+    <t>beddeb2</t>
+  </si>
+  <si>
+    <t>340ee4b</t>
+  </si>
+  <si>
+    <t>9c98d5d</t>
+  </si>
+  <si>
+    <t>64c8ee0</t>
+  </si>
+  <si>
+    <t>b9cc3b3</t>
+  </si>
+  <si>
+    <t>ccd53c8</t>
+  </si>
+  <si>
+    <t>b658ffa</t>
+  </si>
+  <si>
+    <t>e1c8ad4</t>
+  </si>
+  <si>
+    <t>ffd934a</t>
+  </si>
+  <si>
+    <t>3e53dc8</t>
+  </si>
+  <si>
+    <t>d5eee8a</t>
+  </si>
+  <si>
+    <t>77493de</t>
+  </si>
+  <si>
+    <t>6e6486e</t>
+  </si>
+  <si>
+    <t>9870699</t>
+  </si>
+  <si>
+    <t>e2d5d31</t>
+  </si>
+  <si>
+    <t>a7146dd</t>
+  </si>
+  <si>
+    <t>a104ccd</t>
+  </si>
+  <si>
+    <t>3266464</t>
+  </si>
+  <si>
+    <t>ecf376c</t>
+  </si>
+  <si>
+    <t>98a9372</t>
+  </si>
+  <si>
+    <t>d11e988</t>
+  </si>
+  <si>
+    <t>874dbcb</t>
+  </si>
+  <si>
+    <t>6cc0ce0</t>
+  </si>
+  <si>
+    <t>2990709</t>
+  </si>
+  <si>
+    <t>ff65401</t>
+  </si>
+  <si>
+    <t>29d5c0d</t>
+  </si>
+  <si>
+    <t>1bd0eff</t>
+  </si>
+  <si>
+    <t>fca726e</t>
+  </si>
+  <si>
+    <t>27e5c8f</t>
+  </si>
+  <si>
+    <t>63e0d9b</t>
+  </si>
+  <si>
+    <t>df0d4a4</t>
+  </si>
+  <si>
+    <t>0e013b3</t>
+  </si>
+  <si>
+    <t>c2d3592</t>
+  </si>
+  <si>
+    <t>b699acb</t>
+  </si>
+  <si>
+    <t>89bce59</t>
+  </si>
+  <si>
+    <t>550de02</t>
+  </si>
+  <si>
+    <t>83d8cef</t>
+  </si>
+  <si>
+    <t>b173523</t>
+  </si>
+  <si>
+    <t>8b5b8ab</t>
+  </si>
+  <si>
+    <t>2b9a01c</t>
+  </si>
+  <si>
+    <t>19d7406</t>
+  </si>
+  <si>
+    <t>de69d00</t>
+  </si>
+  <si>
+    <t>f1e512d</t>
+  </si>
+  <si>
+    <t>444c960</t>
+  </si>
+  <si>
+    <t>79c49df</t>
+  </si>
+  <si>
+    <t>92f3850</t>
+  </si>
+  <si>
+    <t>2a19576</t>
+  </si>
+  <si>
+    <t>a2f4a85</t>
+  </si>
+  <si>
+    <t>2f18902</t>
+  </si>
+  <si>
+    <t>1c3a76c</t>
+  </si>
+  <si>
+    <t>35d944b</t>
+  </si>
+  <si>
+    <t>e59ebfd</t>
+  </si>
+  <si>
+    <t>993607b</t>
+  </si>
+  <si>
+    <t>aef859c</t>
+  </si>
+  <si>
+    <t>6679e3c</t>
+  </si>
+  <si>
+    <t>c5bdfe3</t>
+  </si>
+  <si>
+    <t>79a2558</t>
+  </si>
+  <si>
+    <t>80e154a</t>
+  </si>
+  <si>
+    <t>94f395e</t>
+  </si>
+  <si>
+    <t>63cac96</t>
+  </si>
+  <si>
+    <t>694e5d0</t>
+  </si>
+  <si>
+    <t>a292054</t>
+  </si>
+  <si>
+    <t>a3c9609</t>
+  </si>
+  <si>
+    <t>fb85e1c</t>
+  </si>
+  <si>
+    <t>32db0dc</t>
+  </si>
+  <si>
+    <t>da999c0</t>
+  </si>
+  <si>
+    <t>43d76b3</t>
+  </si>
+  <si>
+    <t>4a9722c</t>
+  </si>
+  <si>
+    <t>4c35e21</t>
+  </si>
+  <si>
+    <t>2990530</t>
+  </si>
+  <si>
+    <t>84520b9</t>
+  </si>
+  <si>
+    <t>b1fc154</t>
+  </si>
+  <si>
+    <t>6d96013</t>
+  </si>
+  <si>
+    <t>4be4fed</t>
+  </si>
+  <si>
+    <t>4d12ddb</t>
+  </si>
+  <si>
+    <t>020661f</t>
+  </si>
+  <si>
+    <t>60f388e</t>
+  </si>
+  <si>
+    <t>02509eb</t>
+  </si>
+  <si>
+    <t>e28df9d</t>
+  </si>
+  <si>
+    <t>37e5df5</t>
+  </si>
+  <si>
+    <t>33e10d6</t>
+  </si>
+  <si>
+    <t>fe86129</t>
+  </si>
+  <si>
+    <t>7c6f61c</t>
+  </si>
+  <si>
+    <t>5925c9f</t>
+  </si>
+  <si>
+    <t>5410b2d</t>
+  </si>
+  <si>
+    <t>74f741e</t>
+  </si>
+  <si>
+    <t>7ab7fff</t>
+  </si>
+  <si>
+    <t>143ab25</t>
+  </si>
+  <si>
+    <t>17a8334</t>
+  </si>
+  <si>
+    <t>e74ad24</t>
+  </si>
+  <si>
+    <t>325fe57</t>
+  </si>
+  <si>
+    <t>8b9f345</t>
+  </si>
+  <si>
+    <t>38c2666</t>
+  </si>
+  <si>
+    <t>f09933b</t>
+  </si>
+  <si>
+    <t>e3ffee5</t>
+  </si>
+  <si>
+    <t>2599b0c</t>
+  </si>
+  <si>
+    <t>7f53230</t>
+  </si>
+  <si>
+    <t>5ea2077</t>
+  </si>
+  <si>
+    <t>54f686b</t>
+  </si>
+  <si>
+    <t>39b77ae</t>
+  </si>
+  <si>
+    <t>52eafa4</t>
+  </si>
+  <si>
+    <t>aa33aff</t>
+  </si>
+  <si>
+    <t>df7b2d3</t>
+  </si>
+  <si>
+    <t>c405c6a</t>
+  </si>
+  <si>
+    <t>f18753a</t>
+  </si>
+  <si>
+    <t>3877fa9</t>
+  </si>
+  <si>
+    <t>b3403fa</t>
+  </si>
+  <si>
+    <t>a700bc1</t>
+  </si>
+  <si>
+    <t>f539978</t>
+  </si>
+  <si>
+    <t>935f73f</t>
+  </si>
+  <si>
+    <t>dbafdbc</t>
+  </si>
+  <si>
+    <t>c8782eb</t>
+  </si>
+  <si>
+    <t>4e5ade5</t>
+  </si>
+  <si>
+    <t>fc825e9</t>
+  </si>
+  <si>
+    <t>ae16e26</t>
+  </si>
+  <si>
+    <t>5ebf66b</t>
+  </si>
+  <si>
+    <t>51ead85</t>
+  </si>
+  <si>
+    <t>b63b395</t>
+  </si>
+  <si>
+    <t>344d3f4</t>
+  </si>
+  <si>
+    <t>eeb5231</t>
+  </si>
+  <si>
+    <t>8669759</t>
+  </si>
+  <si>
+    <t>8df405e</t>
+  </si>
+  <si>
+    <t>887529c</t>
+  </si>
+  <si>
+    <t>bad2608</t>
+  </si>
+  <si>
+    <t>897dada</t>
+  </si>
+  <si>
+    <t>3fa3da7</t>
+  </si>
+  <si>
+    <t>d485f6c</t>
+  </si>
+  <si>
+    <t>23298ef</t>
+  </si>
+  <si>
+    <t>0087ae9</t>
+  </si>
+  <si>
+    <t>19c9f17</t>
+  </si>
+  <si>
+    <t>b4f83df</t>
+  </si>
+  <si>
+    <t>6d76ef1</t>
+  </si>
+  <si>
+    <t>86158a5</t>
+  </si>
+  <si>
+    <t>d73fb62</t>
+  </si>
+  <si>
+    <t>7e3f6df</t>
+  </si>
+  <si>
+    <t>0c59f17</t>
+  </si>
+  <si>
+    <t>fdf24c6</t>
+  </si>
+  <si>
+    <t>7aca76d</t>
+  </si>
+  <si>
+    <t>b838df9</t>
+  </si>
+  <si>
+    <t>1774f01</t>
+  </si>
+  <si>
+    <t>a7c8e7f</t>
+  </si>
+  <si>
+    <t>030b13d</t>
+  </si>
+  <si>
+    <t>d24b22e</t>
+  </si>
+  <si>
+    <t>1d03e19</t>
+  </si>
+  <si>
+    <t>7a0c892</t>
+  </si>
+  <si>
+    <t>10ca2d1</t>
+  </si>
+  <si>
+    <t>0e7c367</t>
+  </si>
+  <si>
+    <t>ce8b644</t>
+  </si>
+  <si>
+    <t>35670ba</t>
+  </si>
+  <si>
+    <t>fcbc79c</t>
+  </si>
+  <si>
+    <t>f759528</t>
+  </si>
+  <si>
+    <t>a18e571</t>
+  </si>
+  <si>
+    <t>cf25f01</t>
+  </si>
+  <si>
+    <t>b6cf6a3</t>
+  </si>
+  <si>
+    <t>875fb6d</t>
+  </si>
+  <si>
+    <t>e339cad</t>
+  </si>
+  <si>
+    <t>6245ab9</t>
+  </si>
+  <si>
+    <t>b211a4b</t>
+  </si>
+  <si>
+    <t>89dd132</t>
+  </si>
+  <si>
+    <t>802cbea</t>
+  </si>
+  <si>
+    <t>6f45921</t>
+  </si>
+  <si>
+    <t>2e0b118</t>
+  </si>
+  <si>
+    <t>5795e67</t>
+  </si>
+  <si>
+    <t>4d61391</t>
+  </si>
+  <si>
+    <t>e039713</t>
+  </si>
+  <si>
+    <t>8b143f3</t>
+  </si>
+  <si>
+    <t>4beb29d</t>
+  </si>
+  <si>
+    <t>a5e45ce</t>
+  </si>
+  <si>
+    <t>6bb9d5b</t>
+  </si>
+  <si>
+    <t>e0f5542</t>
   </si>
 </sst>
 </file>
@@ -2967,7 +3867,7 @@
     </row>
     <row r="2" spans="1:12" ht="44.25" thickBot="1">
       <c r="A2" s="4" t="s">
-        <v>722</v>
+        <v>1022</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -3006,12 +3906,12 @@
         <v>715</v>
       </c>
       <c r="N2" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="44.25" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>723</v>
+        <v>1023</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -3047,15 +3947,15 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N3" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="58.5" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>724</v>
+        <v>1024</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -3091,15 +3991,15 @@
         <v>23</v>
       </c>
       <c r="M4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N4" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="58.5" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>725</v>
+        <v>1025</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -3135,15 +4035,15 @@
         <v>23</v>
       </c>
       <c r="M5" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N5" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="44.25" thickBot="1">
       <c r="A6" s="4" t="s">
-        <v>726</v>
+        <v>1026</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -3182,12 +4082,12 @@
         <v>715</v>
       </c>
       <c r="N6" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="44.25" thickBot="1">
       <c r="A7" s="7" t="s">
-        <v>727</v>
+        <v>1027</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -3223,15 +4123,15 @@
         <v>23</v>
       </c>
       <c r="M7" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N7" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="44.25" thickBot="1">
       <c r="A8" s="4" t="s">
-        <v>728</v>
+        <v>1028</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -3267,15 +4167,15 @@
         <v>23</v>
       </c>
       <c r="M8" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N8" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="44.25" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>729</v>
+        <v>1029</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -3314,12 +4214,12 @@
         <v>716</v>
       </c>
       <c r="N9" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="58.5" thickBot="1">
       <c r="A10" s="7" t="s">
-        <v>730</v>
+        <v>1030</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -3355,15 +4255,15 @@
         <v>23</v>
       </c>
       <c r="M10" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N10" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="58.5" thickBot="1">
       <c r="A11" s="4" t="s">
-        <v>731</v>
+        <v>1031</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -3402,12 +4302,12 @@
         <v>715</v>
       </c>
       <c r="N11" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="58.5" thickBot="1">
       <c r="A12" s="4" t="s">
-        <v>732</v>
+        <v>1032</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -3443,15 +4343,15 @@
         <v>23</v>
       </c>
       <c r="M12" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N12" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="44.25" thickBot="1">
       <c r="A13" s="7" t="s">
-        <v>733</v>
+        <v>1033</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -3490,12 +4390,12 @@
         <v>715</v>
       </c>
       <c r="N13" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="44.25" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>734</v>
+        <v>1034</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -3531,15 +4431,15 @@
         <v>23</v>
       </c>
       <c r="M14" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N14" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="44.25" thickBot="1">
       <c r="A15" s="4" t="s">
-        <v>735</v>
+        <v>1035</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -3578,12 +4478,12 @@
         <v>715</v>
       </c>
       <c r="N15" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="44.25" thickBot="1">
       <c r="A16" s="7" t="s">
-        <v>736</v>
+        <v>1036</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -3622,12 +4522,12 @@
         <v>715</v>
       </c>
       <c r="N16" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="44.25" thickBot="1">
       <c r="A17" s="4" t="s">
-        <v>737</v>
+        <v>1037</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -3666,12 +4566,12 @@
         <v>715</v>
       </c>
       <c r="N17" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="44.25" thickBot="1">
       <c r="A18" s="4" t="s">
-        <v>738</v>
+        <v>1038</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -3707,15 +4607,15 @@
         <v>23</v>
       </c>
       <c r="M18" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N18" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1">
       <c r="A19" s="7" t="s">
-        <v>739</v>
+        <v>1039</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -3751,15 +4651,15 @@
         <v>23</v>
       </c>
       <c r="M19" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N19" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="44.25" thickBot="1">
       <c r="A20" s="4" t="s">
-        <v>740</v>
+        <v>1040</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -3798,12 +4698,12 @@
         <v>716</v>
       </c>
       <c r="N20" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="44.25" thickBot="1">
       <c r="A21" s="4" t="s">
-        <v>741</v>
+        <v>1041</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -3839,15 +4739,15 @@
         <v>23</v>
       </c>
       <c r="M21" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N21" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="44.25" thickBot="1">
       <c r="A22" s="7" t="s">
-        <v>742</v>
+        <v>1042</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -3883,15 +4783,15 @@
         <v>23</v>
       </c>
       <c r="M22" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N22" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="58.5" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>743</v>
+        <v>1043</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -3930,12 +4830,12 @@
         <v>715</v>
       </c>
       <c r="N23" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="44.25" thickBot="1">
       <c r="A24" s="4" t="s">
-        <v>744</v>
+        <v>1044</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -3979,7 +4879,7 @@
     </row>
     <row r="25" spans="1:12" ht="58.5" thickBot="1">
       <c r="A25" s="7" t="s">
-        <v>745</v>
+        <v>1045</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -4018,12 +4918,12 @@
         <v>716</v>
       </c>
       <c r="N25" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="58.5" thickBot="1">
       <c r="A26" s="4" t="s">
-        <v>746</v>
+        <v>1046</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -4059,15 +4959,15 @@
         <v>23</v>
       </c>
       <c r="M26" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N26" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="58.5" thickBot="1">
       <c r="A27" s="4" t="s">
-        <v>747</v>
+        <v>1047</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -4111,7 +5011,7 @@
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1">
       <c r="A28" s="7" t="s">
-        <v>748</v>
+        <v>1048</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -4150,12 +5050,12 @@
         <v>716</v>
       </c>
       <c r="N28" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1">
       <c r="A29" s="4" t="s">
-        <v>749</v>
+        <v>1049</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -4191,7 +5091,7 @@
         <v>23</v>
       </c>
       <c r="M29" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N29" t="s">
         <v>721</v>
@@ -4199,7 +5099,7 @@
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1">
       <c r="A30" s="4" t="s">
-        <v>750</v>
+        <v>1050</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -4235,15 +5135,15 @@
         <v>23</v>
       </c>
       <c r="M30" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N30" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1">
       <c r="A31" s="7" t="s">
-        <v>751</v>
+        <v>1051</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -4282,12 +5182,12 @@
         <v>715</v>
       </c>
       <c r="N31" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1">
       <c r="A32" s="4" t="s">
-        <v>752</v>
+        <v>1052</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -4323,15 +5223,15 @@
         <v>23</v>
       </c>
       <c r="M32" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N32" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1">
       <c r="A33" s="4" t="s">
-        <v>753</v>
+        <v>1053</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -4370,12 +5270,12 @@
         <v>716</v>
       </c>
       <c r="N33" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1">
       <c r="A34" s="7" t="s">
-        <v>754</v>
+        <v>1054</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -4414,12 +5314,12 @@
         <v>715</v>
       </c>
       <c r="N34" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1">
       <c r="A35" s="4" t="s">
-        <v>755</v>
+        <v>1055</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -4458,12 +5358,12 @@
         <v>715</v>
       </c>
       <c r="N35" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1">
       <c r="A36" s="4" t="s">
-        <v>756</v>
+        <v>1056</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -4499,15 +5399,15 @@
         <v>23</v>
       </c>
       <c r="M36" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N36" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1">
       <c r="A37" s="7" t="s">
-        <v>757</v>
+        <v>1057</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -4543,15 +5443,15 @@
         <v>23</v>
       </c>
       <c r="M37" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N37" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1">
       <c r="A38" s="4" t="s">
-        <v>758</v>
+        <v>1058</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -4590,12 +5490,12 @@
         <v>716</v>
       </c>
       <c r="N38" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1">
       <c r="A39" s="4" t="s">
-        <v>759</v>
+        <v>1059</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -4634,12 +5534,12 @@
         <v>715</v>
       </c>
       <c r="N39" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1">
       <c r="A40" s="7" t="s">
-        <v>760</v>
+        <v>1060</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -4675,15 +5575,15 @@
         <v>23</v>
       </c>
       <c r="M40" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N40" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1">
       <c r="A41" s="4" t="s">
-        <v>761</v>
+        <v>1061</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -4719,15 +5619,15 @@
         <v>23</v>
       </c>
       <c r="M41" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N41" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1">
       <c r="A42" s="4" t="s">
-        <v>762</v>
+        <v>1062</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -4771,7 +5671,7 @@
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1">
       <c r="A43" s="7" t="s">
-        <v>763</v>
+        <v>1063</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -4807,7 +5707,7 @@
         <v>23</v>
       </c>
       <c r="M43" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N43" t="s">
         <v>721</v>
@@ -4815,7 +5715,7 @@
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1">
       <c r="A44" s="4" t="s">
-        <v>764</v>
+        <v>1064</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -4859,7 +5759,7 @@
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1">
       <c r="A45" s="4" t="s">
-        <v>765</v>
+        <v>1065</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -4895,15 +5795,15 @@
         <v>23</v>
       </c>
       <c r="M45" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N45" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1">
       <c r="A46" s="7" t="s">
-        <v>766</v>
+        <v>1066</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -4939,15 +5839,15 @@
         <v>23</v>
       </c>
       <c r="M46" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N46" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1">
       <c r="A47" s="4" t="s">
-        <v>767</v>
+        <v>1067</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -4986,12 +5886,12 @@
         <v>715</v>
       </c>
       <c r="N47" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1">
       <c r="A48" s="4" t="s">
-        <v>768</v>
+        <v>1068</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -5035,7 +5935,7 @@
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1">
       <c r="A49" s="7" t="s">
-        <v>769</v>
+        <v>1069</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -5071,7 +5971,7 @@
         <v>23</v>
       </c>
       <c r="M49" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N49" t="s">
         <v>719</v>
@@ -5079,7 +5979,7 @@
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1">
       <c r="A50" s="4" t="s">
-        <v>770</v>
+        <v>1070</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -5118,12 +6018,12 @@
         <v>715</v>
       </c>
       <c r="N50" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1">
       <c r="A51" s="4" t="s">
-        <v>771</v>
+        <v>1071</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>
@@ -5159,10 +6059,10 @@
         <v>23</v>
       </c>
       <c r="M51" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N51" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited PetStoreMenuTest and page with SoftAssert for links test
</commit_message>
<xml_diff>
--- a/ITBootcamp_Final_Project/data/pet-store-data.xlsx
+++ b/ITBootcamp_Final_Project/data/pet-store-data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3284" uniqueCount="1522">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -3231,6 +3231,1356 @@
   </si>
   <si>
     <t>e0f5542</t>
+  </si>
+  <si>
+    <t>2601283</t>
+  </si>
+  <si>
+    <t>4ec2ac2</t>
+  </si>
+  <si>
+    <t>1b4b003</t>
+  </si>
+  <si>
+    <t>a0b5354</t>
+  </si>
+  <si>
+    <t>c583f66</t>
+  </si>
+  <si>
+    <t>168bf06</t>
+  </si>
+  <si>
+    <t>a5ad401</t>
+  </si>
+  <si>
+    <t>04b8ab9</t>
+  </si>
+  <si>
+    <t>2cfea05</t>
+  </si>
+  <si>
+    <t>baa3960</t>
+  </si>
+  <si>
+    <t>505c1fe</t>
+  </si>
+  <si>
+    <t>8c3c204</t>
+  </si>
+  <si>
+    <t>0d3731d</t>
+  </si>
+  <si>
+    <t>30448b5</t>
+  </si>
+  <si>
+    <t>9ad6c5c</t>
+  </si>
+  <si>
+    <t>26ccab5</t>
+  </si>
+  <si>
+    <t>58e7afd</t>
+  </si>
+  <si>
+    <t>cc909e9</t>
+  </si>
+  <si>
+    <t>4261c34</t>
+  </si>
+  <si>
+    <t>fcee6e6</t>
+  </si>
+  <si>
+    <t>189643a</t>
+  </si>
+  <si>
+    <t>9d7691a</t>
+  </si>
+  <si>
+    <t>523a550</t>
+  </si>
+  <si>
+    <t>cad06c5</t>
+  </si>
+  <si>
+    <t>60e15bf</t>
+  </si>
+  <si>
+    <t>59560ba</t>
+  </si>
+  <si>
+    <t>a3f0667</t>
+  </si>
+  <si>
+    <t>48fca1c</t>
+  </si>
+  <si>
+    <t>d68bb5f</t>
+  </si>
+  <si>
+    <t>3221157</t>
+  </si>
+  <si>
+    <t>abd44d5</t>
+  </si>
+  <si>
+    <t>4177a6c</t>
+  </si>
+  <si>
+    <t>85afe77</t>
+  </si>
+  <si>
+    <t>e2535c1</t>
+  </si>
+  <si>
+    <t>3e8ef81</t>
+  </si>
+  <si>
+    <t>262ae36</t>
+  </si>
+  <si>
+    <t>5e209b2</t>
+  </si>
+  <si>
+    <t>ae8bb82</t>
+  </si>
+  <si>
+    <t>bf57941</t>
+  </si>
+  <si>
+    <t>f296ce3</t>
+  </si>
+  <si>
+    <t>8b229ed</t>
+  </si>
+  <si>
+    <t>32ba760</t>
+  </si>
+  <si>
+    <t>58b3d0d</t>
+  </si>
+  <si>
+    <t>d503411</t>
+  </si>
+  <si>
+    <t>454af8e</t>
+  </si>
+  <si>
+    <t>4aebd42</t>
+  </si>
+  <si>
+    <t>bf54a5c</t>
+  </si>
+  <si>
+    <t>0c42840</t>
+  </si>
+  <si>
+    <t>c1f063c</t>
+  </si>
+  <si>
+    <t>26d9166</t>
+  </si>
+  <si>
+    <t>ffdec89</t>
+  </si>
+  <si>
+    <t>4a02641</t>
+  </si>
+  <si>
+    <t>1c213d1</t>
+  </si>
+  <si>
+    <t>c7c3a4d</t>
+  </si>
+  <si>
+    <t>d190a1f</t>
+  </si>
+  <si>
+    <t>639749a</t>
+  </si>
+  <si>
+    <t>9040ca3</t>
+  </si>
+  <si>
+    <t>b20002a</t>
+  </si>
+  <si>
+    <t>c5a3e12</t>
+  </si>
+  <si>
+    <t>cf3a25b</t>
+  </si>
+  <si>
+    <t>baf1ce5</t>
+  </si>
+  <si>
+    <t>7044a0c</t>
+  </si>
+  <si>
+    <t>9b16cb7</t>
+  </si>
+  <si>
+    <t>6cb4825</t>
+  </si>
+  <si>
+    <t>1b4dd52</t>
+  </si>
+  <si>
+    <t>9949d89</t>
+  </si>
+  <si>
+    <t>b39769a</t>
+  </si>
+  <si>
+    <t>b834f39</t>
+  </si>
+  <si>
+    <t>5fad0cf</t>
+  </si>
+  <si>
+    <t>0140732</t>
+  </si>
+  <si>
+    <t>a582223</t>
+  </si>
+  <si>
+    <t>b6dc11c</t>
+  </si>
+  <si>
+    <t>92fb8bb</t>
+  </si>
+  <si>
+    <t>1f53367</t>
+  </si>
+  <si>
+    <t>ace863f</t>
+  </si>
+  <si>
+    <t>fc8943a</t>
+  </si>
+  <si>
+    <t>fb141b6</t>
+  </si>
+  <si>
+    <t>71b4d76</t>
+  </si>
+  <si>
+    <t>85fb463</t>
+  </si>
+  <si>
+    <t>f560499</t>
+  </si>
+  <si>
+    <t>313b090</t>
+  </si>
+  <si>
+    <t>d68359e</t>
+  </si>
+  <si>
+    <t>05eeab6</t>
+  </si>
+  <si>
+    <t>4c2c12e</t>
+  </si>
+  <si>
+    <t>8cec756</t>
+  </si>
+  <si>
+    <t>6d2bd0e</t>
+  </si>
+  <si>
+    <t>1d88452</t>
+  </si>
+  <si>
+    <t>a70ce2f</t>
+  </si>
+  <si>
+    <t>9bb350f</t>
+  </si>
+  <si>
+    <t>946e5f9</t>
+  </si>
+  <si>
+    <t>71d29fa</t>
+  </si>
+  <si>
+    <t>70afca0</t>
+  </si>
+  <si>
+    <t>de4f764</t>
+  </si>
+  <si>
+    <t>2d16ab5</t>
+  </si>
+  <si>
+    <t>b63a4e3</t>
+  </si>
+  <si>
+    <t>dc18e30</t>
+  </si>
+  <si>
+    <t>23df438</t>
+  </si>
+  <si>
+    <t>3fd9095</t>
+  </si>
+  <si>
+    <t>8c88e74</t>
+  </si>
+  <si>
+    <t>d7d6d10</t>
+  </si>
+  <si>
+    <t>c34205a</t>
+  </si>
+  <si>
+    <t>6044995</t>
+  </si>
+  <si>
+    <t>8558bf8</t>
+  </si>
+  <si>
+    <t>3c5f415</t>
+  </si>
+  <si>
+    <t>18d0161</t>
+  </si>
+  <si>
+    <t>56ad7ae</t>
+  </si>
+  <si>
+    <t>be09662</t>
+  </si>
+  <si>
+    <t>a434907</t>
+  </si>
+  <si>
+    <t>9beac6e</t>
+  </si>
+  <si>
+    <t>8df9ad9</t>
+  </si>
+  <si>
+    <t>8ce20d6</t>
+  </si>
+  <si>
+    <t>d856a40</t>
+  </si>
+  <si>
+    <t>58da3e2</t>
+  </si>
+  <si>
+    <t>f36f5b0</t>
+  </si>
+  <si>
+    <t>7d4e25a</t>
+  </si>
+  <si>
+    <t>c04ebf5</t>
+  </si>
+  <si>
+    <t>f877169</t>
+  </si>
+  <si>
+    <t>23257e1</t>
+  </si>
+  <si>
+    <t>fc78c93</t>
+  </si>
+  <si>
+    <t>ccf0b50</t>
+  </si>
+  <si>
+    <t>ad6ef02</t>
+  </si>
+  <si>
+    <t>2d4e995</t>
+  </si>
+  <si>
+    <t>e397d84</t>
+  </si>
+  <si>
+    <t>e3df33a</t>
+  </si>
+  <si>
+    <t>71c88c0</t>
+  </si>
+  <si>
+    <t>3768e1a</t>
+  </si>
+  <si>
+    <t>3a14478</t>
+  </si>
+  <si>
+    <t>165bbff</t>
+  </si>
+  <si>
+    <t>d77bd59</t>
+  </si>
+  <si>
+    <t>41050ff</t>
+  </si>
+  <si>
+    <t>ab15e36</t>
+  </si>
+  <si>
+    <t>1b20a1c</t>
+  </si>
+  <si>
+    <t>c6eaad8</t>
+  </si>
+  <si>
+    <t>befc5bd</t>
+  </si>
+  <si>
+    <t>8255030</t>
+  </si>
+  <si>
+    <t>b06077b</t>
+  </si>
+  <si>
+    <t>ccc11db</t>
+  </si>
+  <si>
+    <t>8774737</t>
+  </si>
+  <si>
+    <t>d47bcfb</t>
+  </si>
+  <si>
+    <t>f387294</t>
+  </si>
+  <si>
+    <t>01c40af</t>
+  </si>
+  <si>
+    <t>9143c31</t>
+  </si>
+  <si>
+    <t>5961434</t>
+  </si>
+  <si>
+    <t>0378817</t>
+  </si>
+  <si>
+    <t>7d23521</t>
+  </si>
+  <si>
+    <t>a995402</t>
+  </si>
+  <si>
+    <t>66e213e</t>
+  </si>
+  <si>
+    <t>514e55e</t>
+  </si>
+  <si>
+    <t>f19ccce</t>
+  </si>
+  <si>
+    <t>a0415ce</t>
+  </si>
+  <si>
+    <t>20d851c</t>
+  </si>
+  <si>
+    <t>40fe80c</t>
+  </si>
+  <si>
+    <t>02d3234</t>
+  </si>
+  <si>
+    <t>fec3aec</t>
+  </si>
+  <si>
+    <t>8d8b938</t>
+  </si>
+  <si>
+    <t>6a57082</t>
+  </si>
+  <si>
+    <t>1579370</t>
+  </si>
+  <si>
+    <t>f97b35a</t>
+  </si>
+  <si>
+    <t>b381427</t>
+  </si>
+  <si>
+    <t>ee38e64</t>
+  </si>
+  <si>
+    <t>52e937a</t>
+  </si>
+  <si>
+    <t>6798a17</t>
+  </si>
+  <si>
+    <t>d70f79e</t>
+  </si>
+  <si>
+    <t>eef86f3</t>
+  </si>
+  <si>
+    <t>0fd8d0e</t>
+  </si>
+  <si>
+    <t>d8ff1a9</t>
+  </si>
+  <si>
+    <t>50117fc</t>
+  </si>
+  <si>
+    <t>85f8da6</t>
+  </si>
+  <si>
+    <t>925157d</t>
+  </si>
+  <si>
+    <t>fccf4d9</t>
+  </si>
+  <si>
+    <t>535fc10</t>
+  </si>
+  <si>
+    <t>12a688d</t>
+  </si>
+  <si>
+    <t>59e21b4</t>
+  </si>
+  <si>
+    <t>b93b46c</t>
+  </si>
+  <si>
+    <t>02d7554</t>
+  </si>
+  <si>
+    <t>53fd176</t>
+  </si>
+  <si>
+    <t>6c9794f</t>
+  </si>
+  <si>
+    <t>ed136a1</t>
+  </si>
+  <si>
+    <t>20ea930</t>
+  </si>
+  <si>
+    <t>ee6f94f</t>
+  </si>
+  <si>
+    <t>d2c10a6</t>
+  </si>
+  <si>
+    <t>67fc53a</t>
+  </si>
+  <si>
+    <t>5000930</t>
+  </si>
+  <si>
+    <t>f16da33</t>
+  </si>
+  <si>
+    <t>cfa8317</t>
+  </si>
+  <si>
+    <t>7ec0e6d</t>
+  </si>
+  <si>
+    <t>45a9b63</t>
+  </si>
+  <si>
+    <t>fba7ad2</t>
+  </si>
+  <si>
+    <t>22c60d2</t>
+  </si>
+  <si>
+    <t>19b6d5a</t>
+  </si>
+  <si>
+    <t>506b5c6</t>
+  </si>
+  <si>
+    <t>599698b</t>
+  </si>
+  <si>
+    <t>53df52e</t>
+  </si>
+  <si>
+    <t>ad4756e</t>
+  </si>
+  <si>
+    <t>e1ff93c</t>
+  </si>
+  <si>
+    <t>e0ce42c</t>
+  </si>
+  <si>
+    <t>c8d3a9b</t>
+  </si>
+  <si>
+    <t>70704ff</t>
+  </si>
+  <si>
+    <t>0107af4</t>
+  </si>
+  <si>
+    <t>c4c542c</t>
+  </si>
+  <si>
+    <t>60ea6c8</t>
+  </si>
+  <si>
+    <t>403584f</t>
+  </si>
+  <si>
+    <t>5f34497</t>
+  </si>
+  <si>
+    <t>7957b8f</t>
+  </si>
+  <si>
+    <t>376549e</t>
+  </si>
+  <si>
+    <t>90e64c5</t>
+  </si>
+  <si>
+    <t>c5ff2e0</t>
+  </si>
+  <si>
+    <t>24b39da</t>
+  </si>
+  <si>
+    <t>c7cd18d</t>
+  </si>
+  <si>
+    <t>2f98f4d</t>
+  </si>
+  <si>
+    <t>9eaf894</t>
+  </si>
+  <si>
+    <t>3c63886</t>
+  </si>
+  <si>
+    <t>a3147d5</t>
+  </si>
+  <si>
+    <t>3cfe629</t>
+  </si>
+  <si>
+    <t>d0e188c</t>
+  </si>
+  <si>
+    <t>e91531c</t>
+  </si>
+  <si>
+    <t>e1fc5fa</t>
+  </si>
+  <si>
+    <t>63a2818</t>
+  </si>
+  <si>
+    <t>758d4b9</t>
+  </si>
+  <si>
+    <t>80a6bb6</t>
+  </si>
+  <si>
+    <t>7a42ff8</t>
+  </si>
+  <si>
+    <t>aa37da1</t>
+  </si>
+  <si>
+    <t>2416b9f</t>
+  </si>
+  <si>
+    <t>5a93f12</t>
+  </si>
+  <si>
+    <t>1163056</t>
+  </si>
+  <si>
+    <t>d8ef076</t>
+  </si>
+  <si>
+    <t>44a097c</t>
+  </si>
+  <si>
+    <t>2d161a5</t>
+  </si>
+  <si>
+    <t>80eed89</t>
+  </si>
+  <si>
+    <t>15da674</t>
+  </si>
+  <si>
+    <t>a279db4</t>
+  </si>
+  <si>
+    <t>f3da5be</t>
+  </si>
+  <si>
+    <t>a6877df</t>
+  </si>
+  <si>
+    <t>5945480</t>
+  </si>
+  <si>
+    <t>1661950</t>
+  </si>
+  <si>
+    <t>fe04c0d</t>
+  </si>
+  <si>
+    <t>40250a4</t>
+  </si>
+  <si>
+    <t>487004b</t>
+  </si>
+  <si>
+    <t>5a8aabc</t>
+  </si>
+  <si>
+    <t>91b8157</t>
+  </si>
+  <si>
+    <t>b5e159a</t>
+  </si>
+  <si>
+    <t>24b9817</t>
+  </si>
+  <si>
+    <t>1738c85</t>
+  </si>
+  <si>
+    <t>c757d37</t>
+  </si>
+  <si>
+    <t>bf31c41</t>
+  </si>
+  <si>
+    <t>e6d5bd1</t>
+  </si>
+  <si>
+    <t>65356e0</t>
+  </si>
+  <si>
+    <t>75f12e7</t>
+  </si>
+  <si>
+    <t>47cca6c</t>
+  </si>
+  <si>
+    <t>0b0a770</t>
+  </si>
+  <si>
+    <t>11fdbdc</t>
+  </si>
+  <si>
+    <t>50772bf</t>
+  </si>
+  <si>
+    <t>7c0ec51</t>
+  </si>
+  <si>
+    <t>ea4e196</t>
+  </si>
+  <si>
+    <t>9fb89c6</t>
+  </si>
+  <si>
+    <t>189304a</t>
+  </si>
+  <si>
+    <t>8c738f3</t>
+  </si>
+  <si>
+    <t>3afc1d6</t>
+  </si>
+  <si>
+    <t>f41d219</t>
+  </si>
+  <si>
+    <t>c6b6d9b</t>
+  </si>
+  <si>
+    <t>3aa16a0</t>
+  </si>
+  <si>
+    <t>0c76b74</t>
+  </si>
+  <si>
+    <t>95d8386</t>
+  </si>
+  <si>
+    <t>6c00a87</t>
+  </si>
+  <si>
+    <t>437382e</t>
+  </si>
+  <si>
+    <t>699b7e6</t>
+  </si>
+  <si>
+    <t>f96f491</t>
+  </si>
+  <si>
+    <t>db215af</t>
+  </si>
+  <si>
+    <t>bbe835e</t>
+  </si>
+  <si>
+    <t>07918b9</t>
+  </si>
+  <si>
+    <t>00e38e2</t>
+  </si>
+  <si>
+    <t>3f6b2d6</t>
+  </si>
+  <si>
+    <t>84fda87</t>
+  </si>
+  <si>
+    <t>d6adca1</t>
+  </si>
+  <si>
+    <t>7b3950a</t>
+  </si>
+  <si>
+    <t>bf82496</t>
+  </si>
+  <si>
+    <t>860d227</t>
+  </si>
+  <si>
+    <t>8287b47</t>
+  </si>
+  <si>
+    <t>89e8bf6</t>
+  </si>
+  <si>
+    <t>3b63907</t>
+  </si>
+  <si>
+    <t>b3e3ec9</t>
+  </si>
+  <si>
+    <t>089ce55</t>
+  </si>
+  <si>
+    <t>45df889</t>
+  </si>
+  <si>
+    <t>eed40ec</t>
+  </si>
+  <si>
+    <t>f27da3e</t>
+  </si>
+  <si>
+    <t>6d443b1</t>
+  </si>
+  <si>
+    <t>a60708f</t>
+  </si>
+  <si>
+    <t>2a43db9</t>
+  </si>
+  <si>
+    <t>3ee6d42</t>
+  </si>
+  <si>
+    <t>f978eb2</t>
+  </si>
+  <si>
+    <t>28c4d8f</t>
+  </si>
+  <si>
+    <t>c8f39a5</t>
+  </si>
+  <si>
+    <t>63ec9c1</t>
+  </si>
+  <si>
+    <t>1d2acb7</t>
+  </si>
+  <si>
+    <t>51e1b53</t>
+  </si>
+  <si>
+    <t>8d96b35</t>
+  </si>
+  <si>
+    <t>d5d0a45</t>
+  </si>
+  <si>
+    <t>d7c268a</t>
+  </si>
+  <si>
+    <t>439636a</t>
+  </si>
+  <si>
+    <t>277e77f</t>
+  </si>
+  <si>
+    <t>29830b1</t>
+  </si>
+  <si>
+    <t>cc7cf36</t>
+  </si>
+  <si>
+    <t>a148b17</t>
+  </si>
+  <si>
+    <t>2c9c779</t>
+  </si>
+  <si>
+    <t>96cc754</t>
+  </si>
+  <si>
+    <t>7f78888</t>
+  </si>
+  <si>
+    <t>c19a132</t>
+  </si>
+  <si>
+    <t>02918eb</t>
+  </si>
+  <si>
+    <t>cb3ef97</t>
+  </si>
+  <si>
+    <t>cb6a4ca</t>
+  </si>
+  <si>
+    <t>9be1a6e</t>
+  </si>
+  <si>
+    <t>9babc4d</t>
+  </si>
+  <si>
+    <t>4a2ffb1</t>
+  </si>
+  <si>
+    <t>9eeae50</t>
+  </si>
+  <si>
+    <t>a7cab37</t>
+  </si>
+  <si>
+    <t>5f6fcd1</t>
+  </si>
+  <si>
+    <t>81f7b1e</t>
+  </si>
+  <si>
+    <t>7708c70</t>
+  </si>
+  <si>
+    <t>d9e956c</t>
+  </si>
+  <si>
+    <t>e63a450</t>
+  </si>
+  <si>
+    <t>684af6e</t>
+  </si>
+  <si>
+    <t>f6212e8</t>
+  </si>
+  <si>
+    <t>63d0084</t>
+  </si>
+  <si>
+    <t>1601067</t>
+  </si>
+  <si>
+    <t>c4663c0</t>
+  </si>
+  <si>
+    <t>f445dc9</t>
+  </si>
+  <si>
+    <t>605d29f</t>
+  </si>
+  <si>
+    <t>e4db7a2</t>
+  </si>
+  <si>
+    <t>0870769</t>
+  </si>
+  <si>
+    <t>83a58e1</t>
+  </si>
+  <si>
+    <t>67498a8</t>
+  </si>
+  <si>
+    <t>9f2cab0</t>
+  </si>
+  <si>
+    <t>c84770c</t>
+  </si>
+  <si>
+    <t>33e9977</t>
+  </si>
+  <si>
+    <t>e4cfff9</t>
+  </si>
+  <si>
+    <t>4e97473</t>
+  </si>
+  <si>
+    <t>abfefc6</t>
+  </si>
+  <si>
+    <t>93071e7</t>
+  </si>
+  <si>
+    <t>b771571</t>
+  </si>
+  <si>
+    <t>5fa7228</t>
+  </si>
+  <si>
+    <t>e288ac8</t>
+  </si>
+  <si>
+    <t>19f39f0</t>
+  </si>
+  <si>
+    <t>d2da965</t>
+  </si>
+  <si>
+    <t>56e6d32</t>
+  </si>
+  <si>
+    <t>d28d845</t>
+  </si>
+  <si>
+    <t>353acba</t>
+  </si>
+  <si>
+    <t>0a5f8e9</t>
+  </si>
+  <si>
+    <t>d1059be</t>
+  </si>
+  <si>
+    <t>e10b316</t>
+  </si>
+  <si>
+    <t>2c97933</t>
+  </si>
+  <si>
+    <t>b4124f3</t>
+  </si>
+  <si>
+    <t>11ec0ec</t>
+  </si>
+  <si>
+    <t>ce5a150</t>
+  </si>
+  <si>
+    <t>41a6409</t>
+  </si>
+  <si>
+    <t>629d47f</t>
+  </si>
+  <si>
+    <t>ae7be61</t>
+  </si>
+  <si>
+    <t>c678302</t>
+  </si>
+  <si>
+    <t>d9ae203</t>
+  </si>
+  <si>
+    <t>4fd9552</t>
+  </si>
+  <si>
+    <t>76fbae2</t>
+  </si>
+  <si>
+    <t>e0fdedb</t>
+  </si>
+  <si>
+    <t>8419608</t>
+  </si>
+  <si>
+    <t>5ab672a</t>
+  </si>
+  <si>
+    <t>2fc5651</t>
+  </si>
+  <si>
+    <t>9bc6541</t>
+  </si>
+  <si>
+    <t>fb2ba89</t>
+  </si>
+  <si>
+    <t>e52f754</t>
+  </si>
+  <si>
+    <t>2329af1</t>
+  </si>
+  <si>
+    <t>7b7803f</t>
+  </si>
+  <si>
+    <t>4ba118c</t>
+  </si>
+  <si>
+    <t>876c687</t>
+  </si>
+  <si>
+    <t>ab39439</t>
+  </si>
+  <si>
+    <t>cde180f</t>
+  </si>
+  <si>
+    <t>f60717e</t>
+  </si>
+  <si>
+    <t>90991c3</t>
+  </si>
+  <si>
+    <t>cee3042</t>
+  </si>
+  <si>
+    <t>30b542c</t>
+  </si>
+  <si>
+    <t>54efbe5</t>
+  </si>
+  <si>
+    <t>9e31270</t>
+  </si>
+  <si>
+    <t>24c48bb</t>
+  </si>
+  <si>
+    <t>c9c75e7</t>
+  </si>
+  <si>
+    <t>020c195</t>
+  </si>
+  <si>
+    <t>bd9ec8f</t>
+  </si>
+  <si>
+    <t>7b5492b</t>
+  </si>
+  <si>
+    <t>fb49632</t>
+  </si>
+  <si>
+    <t>cefc4b0</t>
+  </si>
+  <si>
+    <t>5263d8b</t>
+  </si>
+  <si>
+    <t>eed2408</t>
+  </si>
+  <si>
+    <t>d594cad</t>
+  </si>
+  <si>
+    <t>b3f47e8</t>
+  </si>
+  <si>
+    <t>87586fa</t>
+  </si>
+  <si>
+    <t>b2dabae</t>
+  </si>
+  <si>
+    <t>72204fe</t>
+  </si>
+  <si>
+    <t>18e7251</t>
+  </si>
+  <si>
+    <t>3445648</t>
+  </si>
+  <si>
+    <t>715e376</t>
+  </si>
+  <si>
+    <t>cd41164</t>
+  </si>
+  <si>
+    <t>21d633d</t>
+  </si>
+  <si>
+    <t>d996fc4</t>
+  </si>
+  <si>
+    <t>6d7446b</t>
+  </si>
+  <si>
+    <t>0d94751</t>
+  </si>
+  <si>
+    <t>19f2049</t>
+  </si>
+  <si>
+    <t>5311690</t>
+  </si>
+  <si>
+    <t>a9b5545</t>
+  </si>
+  <si>
+    <t>58dd74d</t>
+  </si>
+  <si>
+    <t>07bdb8d</t>
+  </si>
+  <si>
+    <t>cfed5dc</t>
+  </si>
+  <si>
+    <t>24aea3a</t>
+  </si>
+  <si>
+    <t>0b026af</t>
+  </si>
+  <si>
+    <t>ca0e083</t>
+  </si>
+  <si>
+    <t>1697c6a</t>
+  </si>
+  <si>
+    <t>c73e5a2</t>
+  </si>
+  <si>
+    <t>1fa0325</t>
+  </si>
+  <si>
+    <t>0614d2b</t>
+  </si>
+  <si>
+    <t>88a29a6</t>
+  </si>
+  <si>
+    <t>e1af405</t>
+  </si>
+  <si>
+    <t>012ed68</t>
+  </si>
+  <si>
+    <t>8fa1a0f</t>
+  </si>
+  <si>
+    <t>231f1d5</t>
+  </si>
+  <si>
+    <t>b296f2b</t>
+  </si>
+  <si>
+    <t>6870f83</t>
+  </si>
+  <si>
+    <t>d2ef047</t>
+  </si>
+  <si>
+    <t>8a8e186</t>
+  </si>
+  <si>
+    <t>e91ea49</t>
+  </si>
+  <si>
+    <t>96a135d</t>
+  </si>
+  <si>
+    <t>6f0f461</t>
+  </si>
+  <si>
+    <t>a51c04c</t>
+  </si>
+  <si>
+    <t>c25733f</t>
+  </si>
+  <si>
+    <t>e2ddb80</t>
+  </si>
+  <si>
+    <t>60f3311</t>
+  </si>
+  <si>
+    <t>f658364</t>
+  </si>
+  <si>
+    <t>4c845b3</t>
+  </si>
+  <si>
+    <t>3556f67</t>
+  </si>
+  <si>
+    <t>306e33c</t>
+  </si>
+  <si>
+    <t>d3e37a4</t>
+  </si>
+  <si>
+    <t>e73b883</t>
+  </si>
+  <si>
+    <t>883875d</t>
+  </si>
+  <si>
+    <t>e640589</t>
+  </si>
+  <si>
+    <t>e543986</t>
+  </si>
+  <si>
+    <t>89aefd2</t>
+  </si>
+  <si>
+    <t>5fb78ae</t>
+  </si>
+  <si>
+    <t>1a65664</t>
+  </si>
+  <si>
+    <t>138adf6</t>
+  </si>
+  <si>
+    <t>43d0f8a</t>
+  </si>
+  <si>
+    <t>586c386</t>
+  </si>
+  <si>
+    <t>79e0726</t>
+  </si>
+  <si>
+    <t>ca8645a</t>
+  </si>
+  <si>
+    <t>2d656ae</t>
+  </si>
+  <si>
+    <t>89b83b5</t>
+  </si>
+  <si>
+    <t>d687cdc</t>
   </si>
 </sst>
 </file>
@@ -3867,7 +5217,7 @@
     </row>
     <row r="2" spans="1:12" ht="44.25" thickBot="1">
       <c r="A2" s="4" t="s">
-        <v>1022</v>
+        <v>1472</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -3903,15 +5253,15 @@
         <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="44.25" thickBot="1">
       <c r="A3" s="4" t="s">
-        <v>1023</v>
+        <v>1473</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -3947,15 +5297,15 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N3" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="58.5" thickBot="1">
       <c r="A4" s="7" t="s">
-        <v>1024</v>
+        <v>1474</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -3994,12 +5344,12 @@
         <v>715</v>
       </c>
       <c r="N4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="58.5" thickBot="1">
       <c r="A5" s="4" t="s">
-        <v>1025</v>
+        <v>1475</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -4038,12 +5388,12 @@
         <v>716</v>
       </c>
       <c r="N5" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="44.25" thickBot="1">
       <c r="A6" s="4" t="s">
-        <v>1026</v>
+        <v>1476</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -4079,15 +5429,15 @@
         <v>23</v>
       </c>
       <c r="M6" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N6" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="44.25" thickBot="1">
       <c r="A7" s="7" t="s">
-        <v>1027</v>
+        <v>1477</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -4123,15 +5473,15 @@
         <v>23</v>
       </c>
       <c r="M7" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N7" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="44.25" thickBot="1">
       <c r="A8" s="4" t="s">
-        <v>1028</v>
+        <v>1478</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -4167,15 +5517,15 @@
         <v>23</v>
       </c>
       <c r="M8" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N8" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="44.25" thickBot="1">
       <c r="A9" s="4" t="s">
-        <v>1029</v>
+        <v>1479</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -4214,12 +5564,12 @@
         <v>716</v>
       </c>
       <c r="N9" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="58.5" thickBot="1">
       <c r="A10" s="7" t="s">
-        <v>1030</v>
+        <v>1480</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -4255,7 +5605,7 @@
         <v>23</v>
       </c>
       <c r="M10" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N10" t="s">
         <v>719</v>
@@ -4263,7 +5613,7 @@
     </row>
     <row r="11" spans="1:12" ht="58.5" thickBot="1">
       <c r="A11" s="4" t="s">
-        <v>1031</v>
+        <v>1481</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -4302,12 +5652,12 @@
         <v>715</v>
       </c>
       <c r="N11" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="58.5" thickBot="1">
       <c r="A12" s="4" t="s">
-        <v>1032</v>
+        <v>1482</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -4343,15 +5693,15 @@
         <v>23</v>
       </c>
       <c r="M12" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N12" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="44.25" thickBot="1">
       <c r="A13" s="7" t="s">
-        <v>1033</v>
+        <v>1483</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -4387,15 +5737,15 @@
         <v>23</v>
       </c>
       <c r="M13" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N13" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="44.25" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>1034</v>
+        <v>1484</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -4431,15 +5781,15 @@
         <v>23</v>
       </c>
       <c r="M14" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N14" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="44.25" thickBot="1">
       <c r="A15" s="4" t="s">
-        <v>1035</v>
+        <v>1485</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -4475,15 +5825,15 @@
         <v>23</v>
       </c>
       <c r="M15" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N15" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="44.25" thickBot="1">
       <c r="A16" s="7" t="s">
-        <v>1036</v>
+        <v>1486</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -4522,12 +5872,12 @@
         <v>715</v>
       </c>
       <c r="N16" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="44.25" thickBot="1">
       <c r="A17" s="4" t="s">
-        <v>1037</v>
+        <v>1487</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -4563,15 +5913,15 @@
         <v>23</v>
       </c>
       <c r="M17" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N17" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="44.25" thickBot="1">
       <c r="A18" s="4" t="s">
-        <v>1038</v>
+        <v>1488</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -4610,12 +5960,12 @@
         <v>716</v>
       </c>
       <c r="N18" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1">
       <c r="A19" s="7" t="s">
-        <v>1039</v>
+        <v>1489</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -4651,15 +6001,15 @@
         <v>23</v>
       </c>
       <c r="M19" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N19" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="44.25" thickBot="1">
       <c r="A20" s="4" t="s">
-        <v>1040</v>
+        <v>1490</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -4698,12 +6048,12 @@
         <v>716</v>
       </c>
       <c r="N20" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="44.25" thickBot="1">
       <c r="A21" s="4" t="s">
-        <v>1041</v>
+        <v>1491</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -4742,12 +6092,12 @@
         <v>716</v>
       </c>
       <c r="N21" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="44.25" thickBot="1">
       <c r="A22" s="7" t="s">
-        <v>1042</v>
+        <v>1492</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -4786,12 +6136,12 @@
         <v>716</v>
       </c>
       <c r="N22" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="58.5" thickBot="1">
       <c r="A23" s="4" t="s">
-        <v>1043</v>
+        <v>1493</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -4835,7 +6185,7 @@
     </row>
     <row r="24" spans="1:12" ht="44.25" thickBot="1">
       <c r="A24" s="4" t="s">
-        <v>1044</v>
+        <v>1494</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -4871,15 +6221,15 @@
         <v>23</v>
       </c>
       <c r="M24" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N24" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="58.5" thickBot="1">
       <c r="A25" s="7" t="s">
-        <v>1045</v>
+        <v>1495</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -4918,12 +6268,12 @@
         <v>716</v>
       </c>
       <c r="N25" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="58.5" thickBot="1">
       <c r="A26" s="4" t="s">
-        <v>1046</v>
+        <v>1496</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -4959,15 +6309,15 @@
         <v>23</v>
       </c>
       <c r="M26" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N26" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="58.5" thickBot="1">
       <c r="A27" s="4" t="s">
-        <v>1047</v>
+        <v>1497</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -5006,12 +6356,12 @@
         <v>716</v>
       </c>
       <c r="N27" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1">
       <c r="A28" s="7" t="s">
-        <v>1048</v>
+        <v>1498</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -5050,12 +6400,12 @@
         <v>716</v>
       </c>
       <c r="N28" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1">
       <c r="A29" s="4" t="s">
-        <v>1049</v>
+        <v>1499</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -5091,15 +6441,15 @@
         <v>23</v>
       </c>
       <c r="M29" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N29" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1">
       <c r="A30" s="4" t="s">
-        <v>1050</v>
+        <v>1500</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -5138,12 +6488,12 @@
         <v>716</v>
       </c>
       <c r="N30" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1">
       <c r="A31" s="7" t="s">
-        <v>1051</v>
+        <v>1501</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -5179,15 +6529,15 @@
         <v>23</v>
       </c>
       <c r="M31" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N31" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1">
       <c r="A32" s="4" t="s">
-        <v>1052</v>
+        <v>1502</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -5226,12 +6576,12 @@
         <v>716</v>
       </c>
       <c r="N32" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1">
       <c r="A33" s="4" t="s">
-        <v>1053</v>
+        <v>1503</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -5270,12 +6620,12 @@
         <v>716</v>
       </c>
       <c r="N33" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1">
       <c r="A34" s="7" t="s">
-        <v>1054</v>
+        <v>1504</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -5319,7 +6669,7 @@
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1">
       <c r="A35" s="4" t="s">
-        <v>1055</v>
+        <v>1505</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -5363,7 +6713,7 @@
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1">
       <c r="A36" s="4" t="s">
-        <v>1056</v>
+        <v>1506</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -5407,7 +6757,7 @@
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1">
       <c r="A37" s="7" t="s">
-        <v>1057</v>
+        <v>1507</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -5446,12 +6796,12 @@
         <v>715</v>
       </c>
       <c r="N37" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1">
       <c r="A38" s="4" t="s">
-        <v>1058</v>
+        <v>1508</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -5487,15 +6837,15 @@
         <v>23</v>
       </c>
       <c r="M38" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N38" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1">
       <c r="A39" s="4" t="s">
-        <v>1059</v>
+        <v>1509</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -5531,15 +6881,15 @@
         <v>23</v>
       </c>
       <c r="M39" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N39" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1">
       <c r="A40" s="7" t="s">
-        <v>1060</v>
+        <v>1510</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -5583,7 +6933,7 @@
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1">
       <c r="A41" s="4" t="s">
-        <v>1061</v>
+        <v>1511</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -5619,15 +6969,15 @@
         <v>23</v>
       </c>
       <c r="M41" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N41" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1">
       <c r="A42" s="4" t="s">
-        <v>1062</v>
+        <v>1512</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -5663,15 +7013,15 @@
         <v>23</v>
       </c>
       <c r="M42" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N42" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1">
       <c r="A43" s="7" t="s">
-        <v>1063</v>
+        <v>1513</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -5710,12 +7060,12 @@
         <v>716</v>
       </c>
       <c r="N43" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1">
       <c r="A44" s="4" t="s">
-        <v>1064</v>
+        <v>1514</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -5751,15 +7101,15 @@
         <v>23</v>
       </c>
       <c r="M44" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N44" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1">
       <c r="A45" s="4" t="s">
-        <v>1065</v>
+        <v>1515</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -5795,7 +7145,7 @@
         <v>23</v>
       </c>
       <c r="M45" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N45" t="s">
         <v>717</v>
@@ -5803,7 +7153,7 @@
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1">
       <c r="A46" s="7" t="s">
-        <v>1066</v>
+        <v>1516</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -5839,15 +7189,15 @@
         <v>23</v>
       </c>
       <c r="M46" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N46" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1">
       <c r="A47" s="4" t="s">
-        <v>1067</v>
+        <v>1517</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -5886,12 +7236,12 @@
         <v>715</v>
       </c>
       <c r="N47" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1">
       <c r="A48" s="4" t="s">
-        <v>1068</v>
+        <v>1518</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -5927,15 +7277,15 @@
         <v>23</v>
       </c>
       <c r="M48" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N48" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1">
       <c r="A49" s="7" t="s">
-        <v>1069</v>
+        <v>1519</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -5971,15 +7321,15 @@
         <v>23</v>
       </c>
       <c r="M49" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="N49" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1">
       <c r="A50" s="4" t="s">
-        <v>1070</v>
+        <v>1520</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -6018,12 +7368,12 @@
         <v>715</v>
       </c>
       <c r="N50" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1">
       <c r="A51" s="4" t="s">
-        <v>1071</v>
+        <v>1521</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>
@@ -6059,7 +7409,7 @@
         <v>23</v>
       </c>
       <c r="M51" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="N51" t="s">
         <v>721</v>

</xml_diff>